<commit_message>
check sda mapping and update the activities
</commit_message>
<xml_diff>
--- a/resource_tracking/prep/hierarchical_service_delivery_area_maps.xlsx
+++ b/resource_tracking/prep/hierarchical_service_delivery_area_maps.xlsx
@@ -10772,8 +10772,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H1521"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView tabSelected="1" topLeftCell="A1494" workbookViewId="0">
+      <selection activeCell="D1524" sqref="D1524"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="32.265625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>